<commit_message>
adding medium info, marker info, and strain names
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_2651.xlsx
+++ b/bioSample/bioSample_2651.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E278CBF-D06A-5D48-BA21-6E73E70D09A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78293F25-9C89-0D42-BD57-E385D72B1955}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14580" yWindow="460" windowWidth="19020" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="66">
   <si>
     <t>harvestDate</t>
   </si>
@@ -215,6 +215,9 @@
   </si>
   <si>
     <t>01.09.18</t>
+  </si>
+  <si>
+    <t>TDY2356</t>
   </si>
 </sst>
 </file>
@@ -580,7 +583,7 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:A45"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -883,6 +886,9 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
+      <c r="E8" t="s">
+        <v>65</v>
+      </c>
       <c r="F8" t="s">
         <v>31</v>
       </c>
@@ -1775,6 +1781,9 @@
       </c>
       <c r="D30" t="s">
         <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>65</v>
       </c>
       <c r="F30" t="s">
         <v>31</v>

</xml_diff>